<commit_message>
Fix: Fixed after feedback
Fix: Fixed after feedback

-Added 2 data sets for airport names and carriers names
- Fixed the feedback issues
</commit_message>
<xml_diff>
--- a/airport-city-code.xlsx
+++ b/airport-city-code.xlsx
@@ -1391,40 +1391,6 @@
   <dxfs count="6">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FFCC0000"/>
-        <name val="Open Sans"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFD1D1D1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1508,13 +1474,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1527,6 +1486,47 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FFCC0000"/>
+        <name val="Open Sans"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFD1D1D1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1543,14 +1543,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="الجدول1" displayName="الجدول1" ref="A1:B191" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="الجدول1" displayName="الجدول1" ref="A1:B191" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <autoFilter ref="A1:B191"/>
   <sortState ref="A2:B191">
     <sortCondition ref="A1:A191"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="CITY" dataDxfId="2"/>
-    <tableColumn id="2" name="Code" dataDxfId="1"/>
+    <tableColumn id="1" name="CITY" dataDxfId="1"/>
+    <tableColumn id="2" name="Code" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1821,8 +1821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80:XFD80"/>
+    <sheetView tabSelected="1" topLeftCell="A186" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3299,7 +3299,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>68</v>
       </c>

</xml_diff>